<commit_message>
::bug:: en el basicNode
</commit_message>
<xml_diff>
--- a/entrega 2 - simio Basemodel/Archivos Auxiliares/distancias asserraderos molinos.xlsx
+++ b/entrega 2 - simio Basemodel/Archivos Auxiliares/distancias asserraderos molinos.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Desktop\Simio\entrega 2 - simio model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Desktop\Simio\entrega 2 - simio Basemodel\Archivos Auxiliares\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="34">
   <si>
     <t>Input@KoalaPesajeEntrada</t>
   </si>
@@ -100,6 +101,33 @@
   <si>
     <t>y8</t>
   </si>
+  <si>
+    <t>DiasDeNoTrabajoAserraderos[</t>
+  </si>
+  <si>
+    <t>,DateTime.DayOfWeek(Run.TimeNow)]</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>DiasDeNoTrabajoAserraderos[100,DateTime.DayOfWeek(Run.TimeNow)]</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>DiasDeNoTrabajoAserraderos[3,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[4,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[7,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[10,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[11,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[15,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[30,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[33,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[34,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[35,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[36,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[38,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[40,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[42,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[45,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[47,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[49,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[50,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[53,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[55,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[60,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[61,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[62,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[67,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[84,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[87,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[88,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[97,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[99,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[100,DateTime.DayOfWeek(Run.TimeNow)]</t>
+  </si>
 </sst>
 </file>
 
@@ -120,15 +148,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,13 +170,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,8 +218,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState ref="A2:R101">
-    <sortCondition ref="R1:R101"/>
+  <sortState ref="A7:R100">
+    <sortCondition ref="A1:A101"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" name="asserradero"/>
@@ -501,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="F2">
-        <f>E2+1</f>
+        <f t="shared" ref="F2:F33" si="0">E2+1</f>
         <v>5</v>
       </c>
       <c r="H2" t="s">
@@ -602,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="1">
-        <f>ABS(D2-I2) + ABS(F2-J2)</f>
+        <f t="shared" ref="L2:L33" si="1">ABS(D2-I2) + ABS(F2-J2)</f>
         <v>2</v>
       </c>
       <c r="N2">
@@ -612,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <f>L2+N2+P2</f>
+        <f t="shared" ref="R2:R33" si="2">L2+N2+P2</f>
         <v>3</v>
       </c>
     </row>
@@ -630,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <f>E3+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H3" t="s">
@@ -643,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="L3" s="1">
-        <f>ABS(D3-I3) + ABS(F3-J3)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N3">
@@ -653,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <f>L3+N3+P3</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -671,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="F4">
-        <f>E4+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H4" t="s">
@@ -684,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="L4" s="1">
-        <f>ABS(D4-I4) + ABS(F4-J4)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N4">
@@ -694,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <f>L4+N4+P4</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -712,7 +761,7 @@
         <v>7</v>
       </c>
       <c r="F5">
-        <f>E5+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H5" t="s">
@@ -725,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="L5">
-        <f>ABS(D5-I5) + ABS(F5-J5)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N5">
@@ -735,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <f>L5+N5+P5</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -753,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <f>E6+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H6" t="s">
@@ -766,7 +815,7 @@
         <v>5</v>
       </c>
       <c r="L6">
-        <f>ABS(D6-I6) + ABS(F6-J6)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="N6">
@@ -776,26 +825,26 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <f>L6+N6+P6</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f>E7+1</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
@@ -808,35 +857,35 @@
       </c>
       <c r="L7">
         <f>ABS(D7-I7) + ABS(F7-J7)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f>L7+N7+P7</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f>E8+1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -847,19 +896,19 @@
       <c r="J8">
         <v>5</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8">
         <f>ABS(D8-I8) + ABS(F8-J8)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R8">
         <f>L8+N8+P8</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -1151,20 +1200,20 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <f>E16+1</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -1177,7 +1226,7 @@
       </c>
       <c r="L16">
         <f>ABS(D16-I16) + ABS(F16-J16)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -1187,7 +1236,7 @@
       </c>
       <c r="R16">
         <f>L16+N16+P16</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -1233,20 +1282,20 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <f>E18+1</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
@@ -1257,9 +1306,9 @@
       <c r="J18">
         <v>5</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18">
         <f>ABS(D18-I18) + ABS(F18-J18)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -1269,7 +1318,7 @@
       </c>
       <c r="R18">
         <f>L18+N18+P18</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -1315,20 +1364,20 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="D20">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <f>E20+1</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H20" t="s">
         <v>4</v>
@@ -1339,19 +1388,22 @@
       <c r="J20">
         <v>5</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20">
         <f>ABS(D20-I20) + ABS(F20-J20)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N20">
         <v>1</v>
       </c>
+      <c r="O20" t="s">
+        <v>10</v>
+      </c>
       <c r="P20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20">
         <f>L20+N20+P20</f>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -1520,20 +1572,20 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <f>E25+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -1546,17 +1598,17 @@
       </c>
       <c r="L25">
         <f>ABS(D25-I25) + ABS(F25-J25)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N25">
         <v>1</v>
       </c>
       <c r="P25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R25">
         <f>L25+N25+P25</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -1766,13 +1818,13 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31">
         <v>3</v>
@@ -1792,7 +1844,7 @@
       </c>
       <c r="L31">
         <f>ABS(D31-I31) + ABS(F31-J31)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -1802,18 +1854,18 @@
       </c>
       <c r="R31">
         <f>L31+N31+P31</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
       </c>
       <c r="D32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1833,13 +1885,13 @@
       </c>
       <c r="L32">
         <f>ABS(D32-I32) + ABS(F32-J32)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N32">
         <v>1</v>
       </c>
       <c r="P32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R32">
         <f>L32+N32+P32</f>
@@ -1848,13 +1900,13 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1874,7 +1926,7 @@
       </c>
       <c r="L33">
         <f>ABS(D33-I33) + ABS(F33-J33)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -1884,7 +1936,7 @@
       </c>
       <c r="R33">
         <f>L33+N33+P33</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -1930,20 +1982,20 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F35">
         <f>E35+1</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H35" t="s">
         <v>4</v>
@@ -1954,15 +2006,15 @@
       <c r="J35">
         <v>5</v>
       </c>
-      <c r="L35" s="1">
+      <c r="L35">
         <f>ABS(D35-I35) + ABS(F35-J35)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N35">
         <v>1</v>
       </c>
       <c r="P35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R35">
         <f>L35+N35+P35</f>
@@ -1971,20 +2023,20 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36">
         <f>E36+1</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H36" t="s">
         <v>4</v>
@@ -1995,19 +2047,19 @@
       <c r="J36">
         <v>5</v>
       </c>
-      <c r="L36" s="1">
+      <c r="L36">
         <f>ABS(D36-I36) + ABS(F36-J36)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P36">
         <v>0</v>
       </c>
       <c r="R36">
         <f>L36+N36+P36</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -2053,20 +2105,20 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F38">
         <f>E38+1</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H38" t="s">
         <v>4</v>
@@ -2077,7 +2129,7 @@
       <c r="J38">
         <v>5</v>
       </c>
-      <c r="L38" s="1">
+      <c r="L38">
         <f>ABS(D38-I38) + ABS(F38-J38)</f>
         <v>5</v>
       </c>
@@ -2135,20 +2187,20 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F40">
         <f>E40+1</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H40" t="s">
         <v>4</v>
@@ -2159,19 +2211,19 @@
       <c r="J40">
         <v>5</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1">
         <f>ABS(D40-I40) + ABS(F40-J40)</f>
         <v>5</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R40">
         <f>L40+N40+P40</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -2381,20 +2433,20 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>2</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F46">
         <f>E46+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H46" t="s">
         <v>4</v>
@@ -2405,9 +2457,9 @@
       <c r="J46">
         <v>5</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="1">
         <f>ABS(D46-I46) + ABS(F46-J46)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -2417,7 +2469,7 @@
       </c>
       <c r="R46">
         <f>L46+N46+P46</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -2463,20 +2515,20 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>2</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F48">
         <f>E48+1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H48" t="s">
         <v>4</v>
@@ -2489,35 +2541,35 @@
       </c>
       <c r="L48" s="1">
         <f>ABS(D48-I48) + ABS(F48-J48)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P48">
         <v>0</v>
       </c>
       <c r="R48">
         <f>L48+N48+P48</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>2</v>
       </c>
       <c r="D49">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49">
         <f>E49+1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H49" t="s">
         <v>4</v>
@@ -2530,7 +2582,7 @@
       </c>
       <c r="L49" s="1">
         <f>ABS(D49-I49) + ABS(F49-J49)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -2540,7 +2592,7 @@
       </c>
       <c r="R49">
         <f>L49+N49+P49</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -2832,20 +2884,20 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
         <v>2</v>
       </c>
       <c r="D57">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E57">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F57">
         <f>E57+1</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H57" t="s">
         <v>4</v>
@@ -2856,19 +2908,19 @@
       <c r="J57">
         <v>5</v>
       </c>
-      <c r="L57">
+      <c r="L57" s="1">
         <f>ABS(D57-I57) + ABS(F57-J57)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57">
         <f>L57+N57+P57</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -3078,20 +3130,20 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
         <v>2</v>
       </c>
       <c r="D63">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F63">
         <f>E63+1</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H63" t="s">
         <v>4</v>
@@ -3102,19 +3154,19 @@
       <c r="J63">
         <v>5</v>
       </c>
-      <c r="L63">
+      <c r="L63" s="1">
         <f>ABS(D63-I63) + ABS(F63-J63)</f>
         <v>4</v>
       </c>
       <c r="N63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R63">
         <f>L63+N63+P63</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -3242,7 +3294,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
@@ -3251,11 +3303,11 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F67">
         <f>E67+1</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H67" t="s">
         <v>4</v>
@@ -3268,17 +3320,17 @@
       </c>
       <c r="L67" s="1">
         <f>ABS(D67-I67) + ABS(F67-J67)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P67">
         <v>0</v>
       </c>
       <c r="R67">
         <f>L67+N67+P67</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -3447,20 +3499,20 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
         <v>2</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E72">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F72">
         <f>E72+1</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H72" t="s">
         <v>4</v>
@@ -3471,19 +3523,19 @@
       <c r="J72">
         <v>5</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="1">
         <f>ABS(D72-I72) + ABS(F72-J72)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R72">
         <f>L72+N72+P72</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -3570,20 +3622,20 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
       </c>
       <c r="D75">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E75">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F75">
         <f>E75+1</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H75" t="s">
         <v>4</v>
@@ -3594,37 +3646,37 @@
       <c r="J75">
         <v>5</v>
       </c>
-      <c r="L75">
+      <c r="L75" s="1">
         <f>ABS(D75-I75) + ABS(F75-J75)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R75">
         <f>L75+N75+P75</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="B76" t="s">
         <v>2</v>
       </c>
       <c r="D76">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E76">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F76">
         <f>E76+1</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H76" t="s">
         <v>4</v>
@@ -3635,37 +3687,37 @@
       <c r="J76">
         <v>5</v>
       </c>
-      <c r="L76">
+      <c r="L76" s="1">
         <f>ABS(D76-I76) + ABS(F76-J76)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R76">
         <f>L76+N76+P76</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
       </c>
       <c r="D77">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E77">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F77">
         <f>E77+1</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H77" t="s">
         <v>4</v>
@@ -3678,17 +3730,17 @@
       </c>
       <c r="L77">
         <f>ABS(D77-I77) + ABS(F77-J77)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N77">
         <v>0</v>
       </c>
       <c r="P77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R77">
         <f>L77+N77+P77</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -3734,20 +3786,20 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
       </c>
       <c r="D79">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F79">
         <f>E79+1</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H79" t="s">
         <v>4</v>
@@ -3760,22 +3812,22 @@
       </c>
       <c r="L79">
         <f>ABS(D79-I79) + ABS(F79-J79)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N79">
         <v>1</v>
       </c>
       <c r="P79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R79">
         <f>L79+N79+P79</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -3784,11 +3836,11 @@
         <v>5</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F80">
         <f>E80+1</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H80" t="s">
         <v>4</v>
@@ -3801,17 +3853,17 @@
       </c>
       <c r="L80">
         <f>ABS(D80-I80) + ABS(F80-J80)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R80">
         <f>L80+N80+P80</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -4226,20 +4278,20 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
         <v>2</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F91">
         <f>E91+1</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H91" t="s">
         <v>4</v>
@@ -4252,35 +4304,35 @@
       </c>
       <c r="L91">
         <f>ABS(D91-I91) + ABS(F91-J91)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="N91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R91">
         <f>L91+N91+P91</f>
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
         <v>2</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F92">
         <f>E92+1</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H92" t="s">
         <v>4</v>
@@ -4293,20 +4345,17 @@
       </c>
       <c r="L92">
         <f>ABS(D92-I92) + ABS(F92-J92)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N92">
-        <v>1</v>
-      </c>
-      <c r="O92" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P92">
         <v>1</v>
       </c>
       <c r="R92">
         <f>L92+N92+P92</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -4434,20 +4483,20 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B96" t="s">
         <v>2</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E96">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F96">
         <f>E96+1</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H96" t="s">
         <v>4</v>
@@ -4458,19 +4507,19 @@
       <c r="J96">
         <v>5</v>
       </c>
-      <c r="L96" s="1">
+      <c r="L96">
         <f>ABS(D96-I96) + ABS(F96-J96)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N96">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R96">
         <f>L96+N96+P96</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -4598,20 +4647,20 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
         <v>2</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E100">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F100">
         <f>E100+1</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H100" t="s">
         <v>4</v>
@@ -4624,17 +4673,17 @@
       </c>
       <c r="L100">
         <f>ABS(D100-I100) + ABS(F100-J100)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P100">
         <v>0</v>
       </c>
       <c r="R100">
         <f>L100+N100+P100</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
@@ -4651,7 +4700,7 @@
         <v>9</v>
       </c>
       <c r="F101">
-        <f>E101+1</f>
+        <f t="shared" ref="F98:F129" si="3">E101+1</f>
         <v>10</v>
       </c>
       <c r="H101" t="s">
@@ -4664,7 +4713,7 @@
         <v>5</v>
       </c>
       <c r="L101">
-        <f>ABS(D101-I101) + ABS(F101-J101)</f>
+        <f t="shared" ref="L66:L101" si="4">ABS(D101-I101) + ABS(F101-J101)</f>
         <v>10</v>
       </c>
       <c r="N101">
@@ -4674,7 +4723,7 @@
         <v>2</v>
       </c>
       <c r="R101">
-        <f>L101+N101+P101</f>
+        <f t="shared" ref="R66:R101" si="5">L101+N101+P101</f>
         <v>12</v>
       </c>
     </row>
@@ -4685,4 +4734,668 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="60.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" s="2">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2">
+        <v>30</v>
+      </c>
+      <c r="H1" s="3">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2">
+        <v>34</v>
+      </c>
+      <c r="J1" s="3">
+        <v>35</v>
+      </c>
+      <c r="K1" s="2">
+        <v>36</v>
+      </c>
+      <c r="L1" s="3">
+        <v>38</v>
+      </c>
+      <c r="M1" s="2">
+        <v>40</v>
+      </c>
+      <c r="N1" s="3">
+        <v>42</v>
+      </c>
+      <c r="O1" s="2">
+        <v>45</v>
+      </c>
+      <c r="P1" s="3">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>49</v>
+      </c>
+      <c r="R1" s="3">
+        <v>50</v>
+      </c>
+      <c r="S1" s="2">
+        <v>53</v>
+      </c>
+      <c r="T1" s="3">
+        <v>55</v>
+      </c>
+      <c r="U1" s="2">
+        <v>60</v>
+      </c>
+      <c r="V1" s="3">
+        <v>61</v>
+      </c>
+      <c r="W1" s="2">
+        <v>62</v>
+      </c>
+      <c r="X1" s="3">
+        <v>67</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>84</v>
+      </c>
+      <c r="Z1" s="3">
+        <v>87</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>88</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>97</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>CONCATENATE(A2,A1,A3)</f>
+        <v>DiasDeNoTrabajoAserraderos[3,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="B4" t="str">
+        <f>CONCATENATE(B2,B1,B3)</f>
+        <v>DiasDeNoTrabajoAserraderos[4,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:AD6" si="0">CONCATENATE(C2,C1,C3)</f>
+        <v>DiasDeNoTrabajoAserraderos[7,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[10,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[11,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[15,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[30,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[33,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[34,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[35,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[36,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[38,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[40,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[42,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[45,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[47,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[49,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[50,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[53,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[55,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[60,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[61,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[62,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[67,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[84,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="Z4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[87,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[88,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[97,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="AC4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[99,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+      <c r="AD4" t="str">
+        <f t="shared" si="0"/>
+        <v>DiasDeNoTrabajoAserraderos[100,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" t="s">
+        <v>27</v>
+      </c>
+      <c r="W5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>CONCATENATE(A4,A5)</f>
+        <v>DiasDeNoTrabajoAserraderos[3,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="B6" t="str">
+        <f>CONCATENATE(B4,B5)</f>
+        <v>DiasDeNoTrabajoAserraderos[4,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="C6" t="str">
+        <f>CONCATENATE(C4,C5)</f>
+        <v>DiasDeNoTrabajoAserraderos[7,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ref="D6:AD6" si="1">CONCATENATE(D4,D5)</f>
+        <v>DiasDeNoTrabajoAserraderos[10,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[11,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[15,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[30,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[33,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[34,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[35,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[36,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[38,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[40,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[42,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[45,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[47,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[49,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[50,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[53,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[55,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[60,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[61,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[62,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[67,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[84,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[87,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[88,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[97,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="AC6" t="str">
+        <f t="shared" si="1"/>
+        <v>DiasDeNoTrabajoAserraderos[99,DateTime.DayOfWeek(Run.TimeNow)]+</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>_xlfn.CONCAT(A6:AD6)</f>
+        <v>DiasDeNoTrabajoAserraderos[3,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[4,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[7,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[10,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[11,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[15,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[30,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[33,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[34,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[35,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[36,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[38,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[40,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[42,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[45,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[47,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[49,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[50,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[53,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[55,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[60,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[61,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[62,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[67,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[84,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[87,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[88,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[97,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[99,DateTime.DayOfWeek(Run.TimeNow)]+DiasDeNoTrabajoAserraderos[100,DateTime.DayOfWeek(Run.TimeNow)]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="str">
+        <f>_xlfn.CONCAT(A9:A12)</f>
+        <v>ABCD</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>